<commit_message>
con conteo de distintas especies por CT
</commit_message>
<xml_diff>
--- a/Tablas informe CT 3.xlsx
+++ b/Tablas informe CT 3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aa631587986ce8df/Documentos/VS Code/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_3F90D48531477C72EA3E833C73B2AA9EDDB3BCCA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E4F9EE4-D0A1-4EB4-924F-D1149403CCD9}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="11_3F90D48531477C72EA3E833C73B2AA9EDDB3BCCA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{862311F2-F63F-4389-A4B9-1B16848FE1BA}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Especie_count" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,25 @@
     <sheet name="freq_by_estacion_binary" sheetId="6" r:id="rId6"/>
     <sheet name="PicturesTaken" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="50">
   <si>
     <t>Especie</t>
   </si>
@@ -173,6 +186,9 @@
   </si>
   <si>
     <t>CT_17</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -180,7 +196,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -207,7 +223,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -243,24 +259,746 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="43">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -291,7 +1029,14 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.0"/>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -301,10 +1046,32 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color auto="1"/>
-        </top>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -320,13 +1087,88 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D23C2A0-8E70-40F7-840C-F44618FBB2C0}" name="Tabla1" displayName="Tabla1" ref="B1:D16" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D23C2A0-8E70-40F7-840C-F44618FBB2C0}" name="Tabla1" displayName="Tabla1" ref="B1:D16" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40">
   <autoFilter ref="B1:D16" xr:uid="{2D23C2A0-8E70-40F7-840C-F44618FBB2C0}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A0C67FFB-EA6B-4479-B43F-B4896375E897}" name="Especie"/>
     <tableColumn id="2" xr3:uid="{B9D5F480-35AD-4F2D-831B-AF9A828F5414}" name="Count"/>
-    <tableColumn id="3" xr3:uid="{8B7D49B2-775E-4CF0-8E44-7F1EBB6E3735}" name="Frequency" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{8B7D49B2-775E-4CF0-8E44-7F1EBB6E3735}" name="Frequency" dataDxfId="39"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C52EE23F-AF6C-4EA9-9315-29614745B527}" name="Tabla2" displayName="Tabla2" ref="B1:J16" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37">
+  <autoFilter ref="B1:J16" xr:uid="{C52EE23F-AF6C-4EA9-9315-29614745B527}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{73748563-6FC6-4A6C-92FA-0E9E5140F124}" name="Especie"/>
+    <tableColumn id="2" xr3:uid="{8DF6BC02-C1CC-49BA-984F-541D635AF244}" name="Araucarias"/>
+    <tableColumn id="3" xr3:uid="{5956143F-5921-4EA7-8661-7C59052F4D15}" name="CoRaTe"/>
+    <tableColumn id="4" xr3:uid="{62BD44C4-AF8E-47BA-BBF0-FB025C2BC482}" name="CoRaTe Quebrada"/>
+    <tableColumn id="5" xr3:uid="{674EB895-E4D4-4B56-AB50-04AEBCC6225A}" name="Lenga"/>
+    <tableColumn id="6" xr3:uid="{B891091C-AD37-4A70-B10A-7F801F8D74F6}" name="Lenga - Pradera"/>
+    <tableColumn id="7" xr3:uid="{E4EE1D72-BC1B-4A52-A84B-B9F1F4DEF5CF}" name="RoRaCo Renoval"/>
+    <tableColumn id="8" xr3:uid="{E882BB5C-16AA-4F5B-B2DD-51DA04E281F7}" name="RoRaCo Río"/>
+    <tableColumn id="9" xr3:uid="{3969ED9B-1AEA-45D0-A46C-D8764BA93422}" name="Santuario de anfibios"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8E5BB5BA-7CF7-4FF6-96A0-1EF16F68FCDD}" name="Tabla3" displayName="Tabla3" ref="B1:J16" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="35" tableBorderDxfId="36" totalsRowBorderDxfId="34">
+  <autoFilter ref="B1:J16" xr:uid="{8E5BB5BA-7CF7-4FF6-96A0-1EF16F68FCDD}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{FFAB8D7B-CD61-486B-9DDF-561DDED971A1}" name="Especie" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{18AC4F1C-2656-42E7-8C14-CC0F9D5E54A8}" name="Araucarias" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{258EF912-596B-406F-AFDA-29EBDF334270}" name="CoRaTe" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{08CF94BE-15EF-44C8-AC9D-8A24F7D4949A}" name="CoRaTe Quebrada" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{DC2D856E-9C68-4684-AACC-A61CFE6F8096}" name="Lenga" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{2DE59C47-E03E-465B-9EC0-5BB2A3E5F558}" name="Lenga - Pradera" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{0FBD26DB-DA16-481D-8623-76E5FCD1E540}" name="RoRaCo Renoval" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{89438BAC-4CFD-4FBD-BAA2-A822CF72F170}" name="RoRaCo Río" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{ADD17D1B-C02F-4360-A1AD-460B2F1D43C7}" name="Santuario de anfibios" dataDxfId="24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6DB83756-116F-4DEB-AAB4-0492FAF43F84}" name="Tabla4" displayName="Tabla4" ref="B1:K17" totalsRowCount="1" headerRowDxfId="20" headerRowBorderDxfId="22" tableBorderDxfId="23" totalsRowBorderDxfId="21">
+  <autoFilter ref="B1:K16" xr:uid="{6DB83756-116F-4DEB-AAB4-0492FAF43F84}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{3D03511F-314E-4A1B-9B15-C1F2B643DEA8}" name="Especie" totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{19B7D297-5BEA-4893-A549-E3A93DC826F0}" name="Araucarias" totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="8">
+      <totalsRowFormula>COUNTIF(Tabla4[Araucarias],"X")</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{C80609EE-A290-4D8D-A06E-5405F530F391}" name="CoRaTe" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="7">
+      <totalsRowFormula>COUNTIF(Tabla4[CoRaTe],"X")</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{E5B890CD-1001-43EB-B1E3-B3305876CBFF}" name="CoRaTe Quebrada" totalsRowFunction="custom" dataDxfId="16" totalsRowDxfId="6">
+      <totalsRowFormula>COUNTIF(Tabla4[CoRaTe Quebrada],"X")</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{29416D2B-8984-40FA-A43E-9571342459A1}" name="Lenga" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="5">
+      <totalsRowFormula>COUNTIF(Tabla4[Lenga],"X")</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{4890D7FC-6685-428A-9717-16F8A5BE20C3}" name="Lenga - Pradera" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="4">
+      <totalsRowFormula>COUNTIF(Tabla4[Lenga - Pradera],"X")</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{BEB74AF9-37AB-461D-91C4-6A89F47B5704}" name="RoRaCo Renoval" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="3">
+      <totalsRowFormula>COUNTIF(Tabla4[RoRaCo Renoval],"X")</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{01BB4EF8-AF59-43B0-82FB-EFD0F635E4F1}" name="RoRaCo Río" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="2">
+      <totalsRowFormula>COUNTIF(Tabla4[RoRaCo Río],"X")</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{AD5E3B95-C74C-4FC3-9FED-E74D8CA9DAA6}" name="Santuario de anfibios" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="1">
+      <totalsRowFormula>COUNTIF(Tabla4[Santuario de anfibios],"X")</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{F99F8685-3568-44BD-AFFB-FE4F385510F5}" name="Percentage" dataDxfId="10" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -621,7 +1463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -864,37 +1706,45 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:J15"/>
+      <selection activeCell="B1" sqref="B1:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="11.06640625" customWidth="1"/>
+    <col min="5" max="5" width="17.1328125" customWidth="1"/>
+    <col min="7" max="7" width="15.1328125" customWidth="1"/>
+    <col min="8" max="8" width="15.796875" customWidth="1"/>
+    <col min="9" max="9" width="11.86328125" customWidth="1"/>
+    <col min="10" max="10" width="19.86328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1380,6 +2230,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1388,7 +2241,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:G15"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1768,7 +2621,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:O15"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2532,44 +3385,47 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:J16"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.06640625" customWidth="1"/>
+    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1328125" customWidth="1"/>
+    <col min="6" max="6" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1328125" customWidth="1"/>
+    <col min="8" max="8" width="15.796875" customWidth="1"/>
+    <col min="9" max="9" width="11.86328125" customWidth="1"/>
+    <col min="10" max="10" width="19.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2577,31 +3433,31 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
+      <c r="C2" s="9">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0</v>
+      </c>
+      <c r="G2" s="9">
+        <v>0</v>
+      </c>
+      <c r="H2" s="9">
         <v>1.4925373134328359</v>
       </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
+      <c r="I2" s="9">
+        <v>0</v>
+      </c>
+      <c r="J2" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2609,31 +3465,31 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9">
         <v>0.74626865671641784</v>
       </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="I3" s="9">
+        <v>0</v>
+      </c>
+      <c r="J3" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2641,31 +3497,31 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0</v>
+      </c>
+      <c r="J4" s="10">
         <v>0.90909090909090906</v>
       </c>
     </row>
@@ -2673,31 +3529,31 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="C5" s="9">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0</v>
+      </c>
+      <c r="J5" s="10">
         <v>0.90909090909090906</v>
       </c>
     </row>
@@ -2705,31 +3561,31 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="9">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9">
         <v>6.0606060606060614</v>
       </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9">
         <v>0.74626865671641784</v>
       </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="I6" s="9">
+        <v>0</v>
+      </c>
+      <c r="J6" s="10">
         <v>1.8181818181818179</v>
       </c>
     </row>
@@ -2737,31 +3593,31 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
+      <c r="C7" s="9">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9">
+        <v>0</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10">
         <v>0.90909090909090906</v>
       </c>
     </row>
@@ -2769,31 +3625,31 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="9">
         <v>9.5238095238095237</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="9">
         <v>18.18181818181818</v>
       </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9">
         <v>9.0909090909090917</v>
       </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2">
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9">
         <v>26.119402985074629</v>
       </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2">
+      <c r="I8" s="9">
+        <v>0</v>
+      </c>
+      <c r="J8" s="10">
         <v>33.636363636363633</v>
       </c>
     </row>
@@ -2801,31 +3657,31 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="9">
         <v>21.428571428571431</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="9">
         <v>18.18181818181818</v>
       </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="9">
         <v>43.18181818181818</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="9">
         <v>50</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="9">
         <v>14.92537313432836</v>
       </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
+      <c r="I9" s="9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="10">
         <v>3.6363636363636358</v>
       </c>
     </row>
@@ -2833,31 +3689,31 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="9">
+        <v>0</v>
+      </c>
+      <c r="D10" s="9">
         <v>15.15151515151515</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="9">
         <v>100</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="9">
         <v>9.0909090909090917</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="9">
         <v>50</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="9">
         <v>26.865671641791049</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="9">
         <v>100</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="10">
         <v>33.636363636363633</v>
       </c>
     </row>
@@ -2865,31 +3721,31 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="9">
         <v>4.7619047619047619</v>
       </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0</v>
+      </c>
+      <c r="J11" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2897,31 +3753,31 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="9">
         <v>11.9047619047619</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="9">
         <v>9.0909090909090917</v>
       </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="E12" s="9">
+        <v>0</v>
+      </c>
+      <c r="F12" s="9">
         <v>9.0909090909090917</v>
       </c>
-      <c r="G12" s="2">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2">
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
+      <c r="H12" s="9">
         <v>2.238805970149254</v>
       </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
+      <c r="I12" s="9">
+        <v>0</v>
+      </c>
+      <c r="J12" s="10">
         <v>1.8181818181818179</v>
       </c>
     </row>
@@ -2929,31 +3785,31 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
+      <c r="C13" s="9">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
         <v>0.74626865671641784</v>
       </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
+      <c r="I13" s="9">
+        <v>0</v>
+      </c>
+      <c r="J13" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2961,31 +3817,31 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="2">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2">
+      <c r="C14" s="9">
+        <v>0</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0</v>
+      </c>
+      <c r="F14" s="9">
+        <v>0</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0</v>
+      </c>
+      <c r="H14" s="9">
         <v>0.74626865671641784</v>
       </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
+      <c r="I14" s="9">
+        <v>0</v>
+      </c>
+      <c r="J14" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2993,31 +3849,31 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="9">
         <v>52.380952380952387</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="9">
         <v>33.333333333333329</v>
       </c>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="E15" s="9">
+        <v>0</v>
+      </c>
+      <c r="F15" s="9">
         <v>29.54545454545455</v>
       </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
+      <c r="G15" s="9">
+        <v>0</v>
+      </c>
+      <c r="H15" s="9">
         <v>25.373134328358208</v>
       </c>
-      <c r="I15" s="2">
-        <v>0</v>
-      </c>
-      <c r="J15" s="2">
+      <c r="I15" s="9">
+        <v>0</v>
+      </c>
+      <c r="J15" s="10">
         <v>20.90909090909091</v>
       </c>
     </row>
@@ -3025,78 +3881,90 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0</v>
-      </c>
-      <c r="J16" s="2">
+      <c r="C16" s="11">
+        <v>0</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0</v>
+      </c>
+      <c r="G16" s="11">
+        <v>0</v>
+      </c>
+      <c r="H16" s="11">
+        <v>0</v>
+      </c>
+      <c r="I16" s="11">
+        <v>0</v>
+      </c>
+      <c r="J16" s="12">
         <v>1.8181818181818179</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="B1:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="11.06640625" customWidth="1"/>
+    <col min="5" max="5" width="17.1328125" customWidth="1"/>
+    <col min="7" max="7" width="15.1328125" customWidth="1"/>
+    <col min="8" max="8" width="15.796875" customWidth="1"/>
+    <col min="9" max="9" width="11.86328125" customWidth="1"/>
+    <col min="10" max="10" width="19.86328125" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3104,13 +3972,20 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K2">
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14">
         <v>12.5</v>
       </c>
     </row>
@@ -3118,13 +3993,20 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K3">
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14">
         <v>12.5</v>
       </c>
     </row>
@@ -3132,13 +4014,20 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J4" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="14">
         <v>12.5</v>
       </c>
     </row>
@@ -3146,13 +4035,20 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J5" t="s">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="14">
         <v>12.5</v>
       </c>
     </row>
@@ -3160,19 +4056,24 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H6" t="s">
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J6" t="s">
+      <c r="I6" s="14"/>
+      <c r="J6" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="14">
         <v>37.5</v>
       </c>
     </row>
@@ -3180,13 +4081,20 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J7" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="14">
         <v>12.5</v>
       </c>
     </row>
@@ -3194,25 +4102,28 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" s="14"/>
+      <c r="F8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" s="14"/>
+      <c r="H8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J8" t="s">
+      <c r="I8" s="14"/>
+      <c r="J8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="14">
         <v>62.5</v>
       </c>
     </row>
@@ -3220,28 +4131,30 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9" s="14"/>
+      <c r="F9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J9" t="s">
+      <c r="I9" s="14"/>
+      <c r="J9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="14">
         <v>75</v>
       </c>
     </row>
@@ -3249,31 +4162,32 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="14">
         <v>87.5</v>
       </c>
     </row>
@@ -3281,13 +4195,20 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K11">
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14">
         <v>12.5</v>
       </c>
     </row>
@@ -3295,25 +4216,28 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12" s="14"/>
+      <c r="F12" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H12" t="s">
+      <c r="G12" s="14"/>
+      <c r="H12" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J12" t="s">
+      <c r="I12" s="14"/>
+      <c r="J12" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="14">
         <v>62.5</v>
       </c>
     </row>
@@ -3321,13 +4245,20 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H13" t="s">
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K13">
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14">
         <v>12.5</v>
       </c>
     </row>
@@ -3335,13 +4266,20 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H14" t="s">
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K14">
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14">
         <v>12.5</v>
       </c>
     </row>
@@ -3349,25 +4287,28 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F15" t="s">
+      <c r="E15" s="14"/>
+      <c r="F15" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H15" t="s">
+      <c r="G15" s="14"/>
+      <c r="H15" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J15" t="s">
+      <c r="I15" s="14"/>
+      <c r="J15" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="14">
         <v>62.5</v>
       </c>
     </row>
@@ -3375,18 +4316,66 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J16" t="s">
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="14">
         <v>12.5</v>
       </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="15">
+        <f>COUNTIF(Tabla4[Araucarias],"X")</f>
+        <v>5</v>
+      </c>
+      <c r="D17" s="15">
+        <f>COUNTIF(Tabla4[CoRaTe],"X")</f>
+        <v>6</v>
+      </c>
+      <c r="E17" s="15">
+        <f>COUNTIF(Tabla4[CoRaTe Quebrada],"X")</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="15">
+        <f>COUNTIF(Tabla4[Lenga],"X")</f>
+        <v>5</v>
+      </c>
+      <c r="G17" s="15">
+        <f>COUNTIF(Tabla4[Lenga - Pradera],"X")</f>
+        <v>2</v>
+      </c>
+      <c r="H17" s="15">
+        <f>COUNTIF(Tabla4[RoRaCo Renoval],"X")</f>
+        <v>10</v>
+      </c>
+      <c r="I17" s="15">
+        <f>COUNTIF(Tabla4[RoRaCo Río],"X")</f>
+        <v>1</v>
+      </c>
+      <c r="J17" s="15">
+        <f>COUNTIF(Tabla4[Santuario de anfibios],"X")</f>
+        <v>10</v>
+      </c>
+      <c r="K17" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -3395,11 +4384,14 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B21" sqref="B21:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="2" max="2" width="11.73046875" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" customWidth="1"/>
+    <col min="4" max="4" width="10.73046875" customWidth="1"/>
     <col min="5" max="5" width="12.06640625" customWidth="1"/>
     <col min="6" max="6" width="14.19921875" customWidth="1"/>
   </cols>

</xml_diff>